<commit_message>
add redux to Filter
</commit_message>
<xml_diff>
--- a/Sergio-shopping-cart.xlsx
+++ b/Sergio-shopping-cart.xlsx
@@ -97,34 +97,34 @@
     <t xml:space="preserve">create a simple backend to send products to front end</t>
   </si>
   <si>
+    <t xml:space="preserve">Add Redux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create store, initial state and reducer and redux devtool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Redux To Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move products state to redux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Redux To Filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move filter state to redux</t>
+  </si>
+  <si>
     <t xml:space="preserve">Active</t>
   </si>
   <si>
-    <t xml:space="preserve">Add Redux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">create store, initial state and reducer and redux devtool</t>
+    <t xml:space="preserve">Add Redux To Cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move cart state to redux</t>
   </si>
   <si>
     <t xml:space="preserve">Open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add Redux To Products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move products state to redux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add Redux To Filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move filter state to redux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add Redux To Cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move cart state to redux</t>
   </si>
   <si>
     <t xml:space="preserve">Create Order</t>
@@ -153,7 +153,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -199,13 +199,6 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -263,7 +256,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -292,15 +285,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,10 +369,10 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.63"/>
@@ -522,176 +507,176 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="6" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="8" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="D11" s="6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="8" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="8" t="n">
+      <c r="D12" s="7" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="8" t="n">
+      <c r="C13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="7" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="8" t="n">
+      <c r="C14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="7" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="8" t="n">
+      <c r="C15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="7" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>